<commit_message>
there are certain errors
</commit_message>
<xml_diff>
--- a/DRM_Results.xlsx
+++ b/DRM_Results.xlsx
@@ -8810,10 +8810,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>209.7957998934633</v>
+        <v>114.7488281915375</v>
       </c>
       <c r="C2" t="n">
-        <v>3743.687908932699</v>
+        <v>3684.157143384041</v>
       </c>
     </row>
     <row r="3">
@@ -8836,10 +8836,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>183.4041512784117</v>
+        <v>278.4511229803375</v>
       </c>
       <c r="C4" t="n">
-        <v>236.8120910673015</v>
+        <v>296.3428566159591</v>
       </c>
     </row>
     <row r="5">
@@ -8849,10 +8849,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>87.42031602708276</v>
+        <v>242.6614087209237</v>
       </c>
       <c r="C5" t="n">
-        <v>6.325636560201811</v>
+        <v>8.043708372975555</v>
       </c>
     </row>
   </sheetData>
@@ -8934,7 +8934,7 @@
         <v>4062</v>
       </c>
       <c r="E2" t="n">
-        <v>4062</v>
+        <v>3587.300048828125</v>
       </c>
       <c r="F2" t="n">
         <v>0.08333333333333333</v>
@@ -8964,7 +8964,7 @@
         <v>4062</v>
       </c>
       <c r="E3" t="n">
-        <v>4062</v>
+        <v>3587.300048828125</v>
       </c>
       <c r="F3" t="n">
         <v>0.08333333333333333</v>
@@ -8994,7 +8994,7 @@
         <v>4062</v>
       </c>
       <c r="E4" t="n">
-        <v>4062</v>
+        <v>3587.300048828125</v>
       </c>
       <c r="F4" t="n">
         <v>0.08333333333333333</v>
@@ -9024,7 +9024,7 @@
         <v>4062</v>
       </c>
       <c r="E5" t="n">
-        <v>4062</v>
+        <v>3587.300048828125</v>
       </c>
       <c r="F5" t="n">
         <v>0.08333333333333333</v>

</xml_diff>